<commit_message>
vault backup: 2025-11-28 00:33:55
</commit_message>
<xml_diff>
--- a/Strumenti.xlsx
+++ b/Strumenti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Public\_Clienti\Maruga\Giochi\Vampiri\Vault\Vampiri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1801BF-2FF5-4BF4-BA58-44C80325C23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7697E92-4897-4AE7-8739-EF232D962609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11124" yWindow="0" windowWidth="31584" windowHeight="16656" activeTab="11" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
+    <workbookView xWindow="9996" yWindow="504" windowWidth="31584" windowHeight="15228" activeTab="8" xr2:uid="{3C69CAEB-EF54-41D7-B74D-5F784B8051C2}"/>
   </bookViews>
   <sheets>
     <sheet name="_Malkavian" sheetId="19" r:id="rId1"/>
@@ -3686,12 +3686,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="49" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="49" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="49" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3711,6 +3705,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="49" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="49" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="49" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -20672,7 +20672,7 @@
   <dimension ref="A1:L225"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C130" sqref="C130"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -22956,6 +22956,9 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CEnrico “Bus” Chiti&amp;R&amp;P/&amp;N</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -23023,23 +23026,23 @@
       <c r="C3" s="39"/>
       <c r="D3" s="36">
         <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E3" s="36">
         <f t="shared" ref="E3:M3" ca="1" si="0">RANDBETWEEN(1,10)</f>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="G3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I3" s="36">
         <f t="shared" ca="1" si="0"/>
@@ -23047,7 +23050,7 @@
       </c>
       <c r="J3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K3" s="36">
         <f t="shared" ca="1" si="0"/>
@@ -23055,11 +23058,11 @@
       </c>
       <c r="L3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="M3" s="36">
         <f t="shared" ca="1" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N3" s="36"/>
     </row>
@@ -23090,39 +23093,39 @@
       </c>
       <c r="E5" s="38">
         <f ca="1">IF(E$3&gt;=$B5,1,0)+D5+IF(E$3=1,-1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F5" s="38">
         <f t="shared" ref="F5:M5" ca="1" si="1">IF(F$3&gt;=$B5,1,0)+E5+IF(F$3=1,-1,0)</f>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="G5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="J5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="K5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="M5" s="38">
         <f t="shared" ca="1" si="1"/>
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:14" x14ac:dyDescent="0.3">
@@ -23136,39 +23139,39 @@
       </c>
       <c r="E6" s="38">
         <f t="shared" ref="E6:M13" ca="1" si="3">IF(E$3&gt;=$B6,1,0)+D6+IF(E$3=1,-1,0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="G6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="M6" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.3">
@@ -23178,43 +23181,43 @@
       <c r="C7" s="39"/>
       <c r="D7" s="38">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="G7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="M7" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.3">
@@ -23224,43 +23227,43 @@
       <c r="C8" s="39"/>
       <c r="D8" s="38">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="G8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M8" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.3">
@@ -23270,43 +23273,43 @@
       <c r="C9" s="39"/>
       <c r="D9" s="38">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="G9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="J9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M9" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.3">
@@ -23316,43 +23319,43 @@
       <c r="C10" s="39"/>
       <c r="D10" s="38">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="G10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="J10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>6</v>
       </c>
       <c r="K10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="L10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="M10" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
@@ -23362,43 +23365,43 @@
       <c r="C11" s="39"/>
       <c r="D11" s="38">
         <f t="shared" ca="1" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>3</v>
       </c>
       <c r="G11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="I11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="J11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="K11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="L11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M11" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
@@ -23412,39 +23415,39 @@
       </c>
       <c r="E12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="G12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="H12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="J12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="K12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="M12" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.3">
@@ -23458,39 +23461,39 @@
       </c>
       <c r="E13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="F13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="G13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="H13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="I13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="J13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="K13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="L13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-2</v>
+        <v>1</v>
       </c>
       <c r="M13" s="38">
         <f t="shared" ca="1" si="3"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.3">
@@ -23513,7 +23516,7 @@
       </c>
       <c r="G16" s="41" cm="1">
         <f t="array" aca="1" ref="G16" ca="1">INDIRECT(ADDRESS(E16+3,D16+3,1))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="4:7" ht="8.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -23529,7 +23532,7 @@
       <c r="F18" s="38"/>
       <c r="G18" s="42" cm="1">
         <f t="array" aca="1" ref="G18" ca="1">INDIRECT(ADDRESS(E18+3,D18+3,1))</f>
-        <v>-1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23542,7 +23545,7 @@
       <c r="F19" s="38"/>
       <c r="G19" s="42" cm="1">
         <f t="array" aca="1" ref="G19" ca="1">INDIRECT(ADDRESS(E19+3,D19+3,1))</f>
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23555,7 +23558,7 @@
       <c r="F20" s="38"/>
       <c r="G20" s="42" cm="1">
         <f t="array" aca="1" ref="G20" ca="1">INDIRECT(ADDRESS(E20+3,D20+3,1))</f>
-        <v>-1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23568,7 +23571,7 @@
       <c r="F21" s="38"/>
       <c r="G21" s="42" cm="1">
         <f t="array" aca="1" ref="G21" ca="1">INDIRECT(ADDRESS(E21+3,D21+3,1))</f>
-        <v>-1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23581,7 +23584,7 @@
       <c r="F22" s="38"/>
       <c r="G22" s="42" cm="1">
         <f t="array" aca="1" ref="G22" ca="1">INDIRECT(ADDRESS(E22+3,D22+3,1))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="4:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -23594,7 +23597,7 @@
       <c r="F23" s="38"/>
       <c r="G23" s="42" cm="1">
         <f t="array" aca="1" ref="G23" ca="1">INDIRECT(ADDRESS(E23+3,D23+3,1))</f>
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -23843,7 +23846,7 @@
   <sheetPr codeName="Foglio4"/>
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -25790,7 +25793,7 @@
   <dimension ref="A1:L225"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -27985,6 +27988,9 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CIrenre Gori&amp;R&amp;P/&amp;N</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -27994,7 +28000,7 @@
   <dimension ref="A1:L225"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -30193,6 +30199,9 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CMarta Fioravanti&amp;R&amp;P/&amp;N</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -30202,7 +30211,7 @@
   <dimension ref="A1:L225"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -32400,6 +32409,9 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CSofia "Rusty" Rinaldi&amp;R&amp;P/&amp;N</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -32409,7 +32421,7 @@
   <dimension ref="A1:L225"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -34610,6 +34622,9 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CMatteo Bechara&amp;R&amp;P/&amp;N</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -34619,7 +34634,7 @@
   <dimension ref="A1:L225"/>
   <sheetViews>
     <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
@@ -36813,6 +36828,9 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;CPaolo Venturi&amp;R&amp;P/&amp;N</oddHeader>
+  </headerFooter>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -41005,7 +41023,7 @@
   </sheetPr>
   <dimension ref="A1:S61"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="U9" sqref="U9"/>
     </sheetView>
   </sheetViews>
@@ -41020,42 +41038,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
-      <c r="A1" s="219" t="s">
+      <c r="A1" s="217" t="s">
         <v>390</v>
       </c>
-      <c r="B1" s="219"/>
-      <c r="C1" s="219"/>
-      <c r="D1" s="219"/>
-      <c r="E1" s="219"/>
-      <c r="F1" s="219"/>
-      <c r="G1" s="219"/>
-      <c r="H1" s="219"/>
-      <c r="I1" s="219"/>
-      <c r="J1" s="220">
+      <c r="B1" s="217"/>
+      <c r="C1" s="217"/>
+      <c r="D1" s="217"/>
+      <c r="E1" s="217"/>
+      <c r="F1" s="217"/>
+      <c r="G1" s="217"/>
+      <c r="H1" s="217"/>
+      <c r="I1" s="217"/>
+      <c r="J1" s="218">
         <f>C7</f>
         <v>0.8125</v>
       </c>
-      <c r="K1" s="221"/>
-      <c r="L1" s="213">
+      <c r="K1" s="219"/>
+      <c r="L1" s="220">
         <f>C8</f>
         <v>0.83333333333333337</v>
       </c>
-      <c r="M1" s="221"/>
-      <c r="N1" s="213">
+      <c r="M1" s="219"/>
+      <c r="N1" s="220">
         <f>C9</f>
         <v>0.85416666666666674</v>
       </c>
-      <c r="O1" s="221"/>
-      <c r="P1" s="213">
+      <c r="O1" s="219"/>
+      <c r="P1" s="220">
         <f>C10</f>
         <v>0.87500000000000011</v>
       </c>
-      <c r="Q1" s="221"/>
-      <c r="R1" s="213">
+      <c r="Q1" s="219"/>
+      <c r="R1" s="220">
         <f>C11</f>
         <v>0.89583333333333348</v>
       </c>
-      <c r="S1" s="214"/>
+      <c r="S1" s="221"/>
     </row>
     <row r="2" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="J2" s="176"/>
@@ -41138,31 +41156,31 @@
       <c r="F6" s="4" t="s">
         <v>389</v>
       </c>
-      <c r="J6" s="215">
+      <c r="J6" s="213">
         <f>C12</f>
         <v>0.91666666666666685</v>
       </c>
-      <c r="K6" s="216"/>
-      <c r="L6" s="217">
+      <c r="K6" s="214"/>
+      <c r="L6" s="215">
         <f>C13</f>
         <v>0.93750000000000022</v>
       </c>
-      <c r="M6" s="216"/>
-      <c r="N6" s="217">
+      <c r="M6" s="214"/>
+      <c r="N6" s="215">
         <f>C14</f>
         <v>0.95833333333333359</v>
       </c>
-      <c r="O6" s="216"/>
-      <c r="P6" s="217">
+      <c r="O6" s="214"/>
+      <c r="P6" s="215">
         <f>C15</f>
         <v>0.97916666666666696</v>
       </c>
-      <c r="Q6" s="216"/>
-      <c r="R6" s="217">
+      <c r="Q6" s="214"/>
+      <c r="R6" s="215">
         <f>C16</f>
         <v>1.0000000000000002</v>
       </c>
-      <c r="S6" s="218"/>
+      <c r="S6" s="216"/>
     </row>
     <row r="7" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="A7" s="4" t="s">
@@ -41300,31 +41318,31 @@
       <c r="F11" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="J11" s="215">
+      <c r="J11" s="213">
         <f>C17</f>
         <v>1.0208333333333335</v>
       </c>
-      <c r="K11" s="216"/>
-      <c r="L11" s="217">
+      <c r="K11" s="214"/>
+      <c r="L11" s="215">
         <f>C18</f>
         <v>1.0416666666666667</v>
       </c>
-      <c r="M11" s="216"/>
-      <c r="N11" s="217">
+      <c r="M11" s="214"/>
+      <c r="N11" s="215">
         <f>C19</f>
         <v>1.0625</v>
       </c>
-      <c r="O11" s="216"/>
-      <c r="P11" s="217">
+      <c r="O11" s="214"/>
+      <c r="P11" s="215">
         <f>C20</f>
         <v>1.0833333333333333</v>
       </c>
-      <c r="Q11" s="216"/>
-      <c r="R11" s="217">
+      <c r="Q11" s="214"/>
+      <c r="R11" s="215">
         <f>C21</f>
         <v>1.1041666666666665</v>
       </c>
-      <c r="S11" s="218"/>
+      <c r="S11" s="216"/>
     </row>
     <row r="12" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B12" s="173">
@@ -41454,31 +41472,31 @@
       <c r="E16" s="3" t="s">
         <v>375</v>
       </c>
-      <c r="J16" s="215">
+      <c r="J16" s="213">
         <f>C22</f>
         <v>1.1249999999999998</v>
       </c>
-      <c r="K16" s="216"/>
-      <c r="L16" s="217">
+      <c r="K16" s="214"/>
+      <c r="L16" s="215">
         <f>C23</f>
         <v>1.145833333333333</v>
       </c>
-      <c r="M16" s="216"/>
-      <c r="N16" s="217">
+      <c r="M16" s="214"/>
+      <c r="N16" s="215">
         <f>C24</f>
         <v>1.1666666666666663</v>
       </c>
-      <c r="O16" s="216"/>
-      <c r="P16" s="217">
+      <c r="O16" s="214"/>
+      <c r="P16" s="215">
         <f>C25</f>
         <v>1.1874999999999996</v>
       </c>
-      <c r="Q16" s="216"/>
-      <c r="R16" s="217">
+      <c r="Q16" s="214"/>
+      <c r="R16" s="215">
         <f>C26</f>
         <v>1.2083333333333328</v>
       </c>
-      <c r="S16" s="218"/>
+      <c r="S16" s="216"/>
     </row>
     <row r="17" spans="1:19" ht="18.600000000000001" x14ac:dyDescent="0.4">
       <c r="B17" s="173">
@@ -41614,31 +41632,31 @@
       <c r="F21" s="4" t="s">
         <v>387</v>
       </c>
-      <c r="J21" s="215">
+      <c r="J21" s="213">
         <f>C27</f>
         <v>1.2291666666666661</v>
       </c>
-      <c r="K21" s="216"/>
-      <c r="L21" s="217">
+      <c r="K21" s="214"/>
+      <c r="L21" s="215">
         <f>C28</f>
         <v>1.2499999999999993</v>
       </c>
-      <c r="M21" s="216"/>
-      <c r="N21" s="217">
+      <c r="M21" s="214"/>
+      <c r="N21" s="215">
         <f>C29</f>
         <v>1.2708333333333326</v>
       </c>
-      <c r="O21" s="216"/>
-      <c r="P21" s="217">
+      <c r="O21" s="214"/>
+      <c r="P21" s="215">
         <f>C30</f>
         <v>1.2916666666666659</v>
       </c>
-      <c r="Q21" s="216"/>
-      <c r="R21" s="217">
+      <c r="Q21" s="214"/>
+      <c r="R21" s="215">
         <f>C31</f>
         <v>1.3124999999999991</v>
       </c>
-      <c r="S21" s="218"/>
+      <c r="S21" s="216"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.35">
       <c r="B22" s="173">
@@ -42367,11 +42385,18 @@
     </row>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="J21:K21"/>
-    <mergeCell ref="L21:M21"/>
-    <mergeCell ref="N21:O21"/>
-    <mergeCell ref="P21:Q21"/>
-    <mergeCell ref="R21:S21"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="N6:O6"/>
+    <mergeCell ref="P6:Q6"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="R11:S11"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L16:M16"/>
+    <mergeCell ref="N16:O16"/>
+    <mergeCell ref="P16:Q16"/>
+    <mergeCell ref="R16:S16"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="J11:K11"/>
     <mergeCell ref="L11:M11"/>
@@ -42381,18 +42406,11 @@
     <mergeCell ref="L1:M1"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R11:S11"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L16:M16"/>
-    <mergeCell ref="N16:O16"/>
-    <mergeCell ref="P16:Q16"/>
-    <mergeCell ref="R16:S16"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="N6:O6"/>
-    <mergeCell ref="P6:Q6"/>
-    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="L21:M21"/>
+    <mergeCell ref="N21:O21"/>
+    <mergeCell ref="P21:Q21"/>
+    <mergeCell ref="R21:S21"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>